<commit_message>
Skill system / PlayerCardPage
</commit_message>
<xml_diff>
--- a/LarpCreater/LARP Framework/Assets/Excel/Skill.xlsx
+++ b/LarpCreater/LARP Framework/Assets/Excel/Skill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LARP_System\LarpCreater\LARP Framework\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F44BA52-A04F-4F30-ACEC-E8FB54FD40B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA9E2E-EE36-4365-9A44-4F7FDFA36C84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="5540" windowWidth="30670" windowHeight="15460" xr2:uid="{BD68BDBC-1884-4FFC-85E7-D31DC8E6B5B9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
   <si>
     <t>招式名字</t>
     <phoneticPr fontId="1"/>
@@ -457,6 +457,10 @@
   </si>
   <si>
     <t>無限</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>系列最大點數</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -875,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D31EB2-6EDA-46D2-9AC9-0993C18F3522}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -887,7 +891,7 @@
     <col min="5" max="5" width="59.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -921,8 +925,11 @@
       <c r="K1" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -941,8 +948,11 @@
       <c r="K2" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -961,8 +971,11 @@
       <c r="K3" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -981,8 +994,11 @@
       <c r="K4" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1001,8 +1017,11 @@
       <c r="K5" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1021,8 +1040,11 @@
       <c r="K6" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1044,8 +1066,11 @@
       <c r="K7" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1067,8 +1092,11 @@
       <c r="K8" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1087,8 +1115,11 @@
       <c r="K9" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1110,8 +1141,11 @@
       <c r="K10" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1130,8 +1164,11 @@
       <c r="K11" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1150,8 +1187,11 @@
       <c r="K12" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -1170,8 +1210,11 @@
       <c r="K13" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -1190,8 +1233,11 @@
       <c r="K14" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1210,8 +1256,11 @@
       <c r="K15" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -1233,8 +1282,11 @@
       <c r="K16" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -1256,8 +1308,11 @@
       <c r="K17" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1276,8 +1331,11 @@
       <c r="K18" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1302,8 +1360,11 @@
       <c r="K19" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1328,8 +1389,11 @@
       <c r="K20" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -1354,8 +1418,11 @@
       <c r="K21" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1374,8 +1441,11 @@
       <c r="K22" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1394,8 +1464,11 @@
       <c r="K23" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1417,8 +1490,11 @@
       <c r="K24" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -1440,8 +1516,11 @@
       <c r="K25" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -1460,8 +1539,11 @@
       <c r="K26" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
@@ -1480,8 +1562,11 @@
       <c r="K27" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1500,8 +1585,11 @@
       <c r="K28" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -1520,8 +1608,11 @@
       <c r="K29" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -1540,8 +1631,11 @@
       <c r="K30" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -1560,12 +1654,16 @@
       <c r="K31" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="E32" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>